<commit_message>
minor adaptations in R Lecture
</commit_message>
<xml_diff>
--- a/AssignmentCreditsDSMWS1718.xlsx
+++ b/AssignmentCreditsDSMWS1718.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Python Assigments</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Data Types</t>
+  </si>
+  <si>
+    <t>Visualisation</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B18"/>
+  <dimension ref="A2:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,6 +539,14 @@
       </c>
       <c r="B18">
         <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor adaptations in R lectures
</commit_message>
<xml_diff>
--- a/AssignmentCreditsDSMWS1718.xlsx
+++ b/AssignmentCreditsDSMWS1718.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Python Assigments</t>
   </si>
@@ -411,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B19"/>
+  <dimension ref="A2:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,6 +546,22 @@
         <v>15</v>
       </c>
       <c r="B19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
         <v>15</v>
       </c>
     </row>

</xml_diff>